<commit_message>
unhide columns and update fields
</commit_message>
<xml_diff>
--- a/templates/data-templates/2020-11_data_event.xlsx
+++ b/templates/data-templates/2020-11_data_event.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biodiversityaq/Desktop/data-mgt-templates/templates/data-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF62055C-CE23-D347-9797-84FB8AC1E783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E7A446-3567-974D-A7CD-F4C4AF271AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>eventID</t>
   </si>
@@ -66,9 +66,6 @@
     <t>geodeticDatum</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>timeZone</t>
   </si>
   <si>
@@ -82,6 +79,18 @@
   </si>
   <si>
     <t>eventRemarks</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>eventTime</t>
   </si>
 </sst>
 </file>
@@ -451,24 +460,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="19.6640625" style="1"/>
-    <col min="5" max="7" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="11" width="19.6640625" style="1"/>
-    <col min="12" max="14" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" style="1"/>
-    <col min="16" max="16" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="16384" width="19.6640625" style="1"/>
+    <col min="1" max="8" width="19.6640625" style="1"/>
+    <col min="9" max="9" width="19.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16" width="19.6640625" style="1"/>
+    <col min="17" max="17" width="17" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="19.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -479,46 +491,55 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>